<commit_message>
Working Ecorp but might not be enough in gitignore
How does the handoff of Ecorp to Batchdata look? Up next: Perhaps removing all documentation within agent_ecorp so it's fully absorbed into main pipeline.
</commit_message>
<xml_diff>
--- a/ecorp/agent_ecorp/v2EDITTED8.25 copy.xlsx
+++ b/ecorp/agent_ecorp/v2EDITTED8.25 copy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrettsullivan/Desktop/agent_ecorp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrettsullivan/Desktop/BHRF/Data_Recourses/LANDSCRAPE/adhs-restore-28-Jul-2025 copy/Ecorp/agent_ecorp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F6732D-F3B7-074A-ACFE-CA2657D3EA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F82EB0C-6112-2E4E-ADC4-E69619BFB286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17800" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="500" windowWidth="17800" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -517,7 +517,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -825,9 +825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>